<commit_message>
fix bug in string to 3d repr (infinite loop)
</commit_message>
<xml_diff>
--- a/_garbage/input_string_matrix_to_array.xlsx
+++ b/_garbage/input_string_matrix_to_array.xlsx
@@ -105,7 +105,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +117,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -142,9 +149,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,7 +436,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,7 +460,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
@@ -465,7 +473,7 @@
         <v>5</v>
       </c>
       <c r="E2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -479,7 +487,7 @@
       </c>
       <c r="I2" s="1">
         <f>D2*9+E2</f>
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="J2" s="1">
         <f>F2*9+G2</f>
@@ -487,11 +495,11 @@
       </c>
       <c r="L2" t="str">
         <f>CONCATENATE("input[",H2,"] + input[",I2,"] + input[",J2,"],")</f>
-        <v>input[2] + input[53] + input[11],</v>
+        <v>input[2] + input[45] + input[11],</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3">
@@ -530,7 +538,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4">
@@ -569,7 +577,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5">
@@ -608,7 +616,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6">
@@ -686,7 +694,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8">
@@ -725,7 +733,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9">

</xml_diff>